<commit_message>
v.1.2 year analysis developed, new plots added
</commit_message>
<xml_diff>
--- a/data/monthly/2099.01.xlsx
+++ b/data/monthly/2099.01.xlsx
@@ -576,6 +576,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+kebab</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1348,7 +1372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1359,7 +1383,7 @@
   <dimension ref="A1:AA140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1388,7 +1412,7 @@
       </c>
       <c r="B1" s="31">
         <f>E1-A9</f>
-        <v>1990.5</v>
+        <v>1975.5</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>11</v>
@@ -1415,7 +1439,7 @@
       </c>
       <c r="B2" s="32">
         <f>E2-A9</f>
-        <v>1855.5</v>
+        <v>1840.5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="12" t="s">
@@ -1548,7 +1572,7 @@
     <row r="6" spans="1:27" ht="15.75" thickBot="1">
       <c r="A6" s="28">
         <f>SUM(B9+C9+D9+F9+E9+G9)</f>
-        <v>1890.5</v>
+        <v>1905.5</v>
       </c>
       <c r="B6" s="29">
         <f>SUM(H9+J9+K9+I9+L9+N9+P9+O9)</f>
@@ -1607,35 +1631,35 @@
       </c>
       <c r="B8" s="6">
         <f t="shared" ref="B8:T8" si="0">100*B9/$A$9</f>
-        <v>25.337206889396139</v>
+        <v>25.799133842029285</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>37.35214774849554</v>
+        <v>37.12105588781192</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>8.0514629591201494</v>
+        <v>8.0016498247061243</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ref="E8:K8" si="1">100*E9/$A$9</f>
-        <v>0.99605727329321436</v>
+        <v>0.98989482367498449</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="1"/>
-        <v>4.8557792073044199</v>
+        <v>4.8257372654155493</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="1"/>
-        <v>1.8676073874247769</v>
+        <v>1.856052794390596</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="1"/>
-        <v>5.1462959120149412</v>
+        <v>5.1144565889874203</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="1"/>
-        <v>14.525835235526042</v>
+        <v>14.435966178593524</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="1"/>
@@ -1651,7 +1675,7 @@
       </c>
       <c r="M8" s="6">
         <f t="shared" ref="M8:S8" si="2">100*M9/$A$9</f>
-        <v>0.83004772774434532</v>
+        <v>0.82491235306248711</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="2"/>
@@ -1663,7 +1687,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>1.0375596596804317</v>
+        <v>1.0311404413281089</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="2"/>
@@ -1685,11 +1709,11 @@
     <row r="9" spans="1:27" ht="15.75" thickBot="1">
       <c r="A9" s="5">
         <f>SUM(B9:Z9)</f>
-        <v>2409.5</v>
+        <v>2424.5</v>
       </c>
       <c r="B9" s="16">
         <f>SUM(B11:B706)</f>
-        <v>610.5</v>
+        <v>625.5</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" ref="C9:R9" si="3">SUM(C11:C706)</f>
@@ -2012,7 +2036,9 @@
       <c r="A17" s="13">
         <v>7</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="19">
+        <v>15</v>
+      </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>

</xml_diff>